<commit_message>
Corrección pts puche clasf
</commit_message>
<xml_diff>
--- a/data/clasf_jor7_gB.xlsx
+++ b/data/clasf_jor7_gB.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{185C8498-1228-4463-B07B-E9E54439F831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F101587-772D-42FC-844B-F7A3342CB7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$7</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -63,13 +66,13 @@
     <t>Armada</t>
   </si>
   <si>
+    <t>Puche</t>
+  </si>
+  <si>
     <t>Gonzo</t>
   </si>
   <si>
     <t>Coquina</t>
-  </si>
-  <si>
-    <t>Puche</t>
   </si>
   <si>
     <t>Kike</t>
@@ -438,7 +441,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -526,22 +529,22 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>7</v>
@@ -555,10 +558,10 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -578,22 +581,22 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
         <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
       </c>
       <c r="H6">
         <v>7</v>
@@ -626,6 +629,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H7" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H7">
+      <sortCondition descending="1" ref="B1:B7"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>